<commit_message>
remove search functionality, not needed
</commit_message>
<xml_diff>
--- a/Report Files/functional spec/Gantt.xlsx
+++ b/Report Files/functional spec/Gantt.xlsx
@@ -12,7 +12,6 @@
     <sheet name="Ark3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -1601,8 +1600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AP38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="X21" sqref="X21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Y21" sqref="Y21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2759,7 +2758,7 @@
       <c r="V21" s="70"/>
       <c r="W21" s="70"/>
       <c r="X21" s="59"/>
-      <c r="Y21" s="65"/>
+      <c r="Y21" s="59"/>
       <c r="Z21" s="51"/>
       <c r="AA21" s="51"/>
       <c r="AB21" s="51"/>

</xml_diff>

<commit_message>
remove news.html and replace with launch.html
</commit_message>
<xml_diff>
--- a/Report Files/functional spec/Gantt.xlsx
+++ b/Report Files/functional spec/Gantt.xlsx
@@ -1601,7 +1601,7 @@
   <dimension ref="A1:AP38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AR12" sqref="AR12"/>
+      <selection activeCell="AV13" sqref="AV13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2764,7 +2764,7 @@
       <c r="AB21" s="59"/>
       <c r="AC21" s="59"/>
       <c r="AD21" s="59"/>
-      <c r="AE21" s="51"/>
+      <c r="AE21" s="59"/>
       <c r="AF21" s="51"/>
       <c r="AG21" s="51"/>
       <c r="AH21" s="51"/>

</xml_diff>